<commit_message>
Prune startup.sh container scripts
</commit_message>
<xml_diff>
--- a/bikesharing_output/kpis.xlsx
+++ b/bikesharing_output/kpis.xlsx
@@ -646,19 +646,19 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>B00514 (21)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>B00539 (21)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>B00454 (21)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>B00539 (21)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>B00514 (21)</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>B00316 (20)</t>
@@ -666,17 +666,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>B00159 (20)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>B00358 (20)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>B00557 (20)</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>B00358 (20)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>B00159 (20)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -842,22 +842,22 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>B00021 (109)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>B00206 (109)</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>B00021 (109)</t>
-        </is>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>B00120 (108)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>B00144 (108)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>B00120 (108)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -1184,14 +1184,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>B00217 (102)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>B00078 (102)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>B00217 (102)</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>B00272 (102)</t>
@@ -1214,12 +1214,12 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
+          <t>B00109 (94)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
           <t>B00127 (94)</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>B00109 (94)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1370,27 +1370,27 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
+          <t>B00311 (73)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
           <t>B00121 (73)</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>B00311 (73)</t>
-        </is>
-      </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>B00353 (72)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>B00289 (72)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>B00431 (72)</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>B00289 (72)</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>B00353 (72)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1747,29 +1747,29 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>B00149 (60)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>B00125 (60)</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>B00149 (60)</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>B00008 (59)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>B00389 (59)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>B00101 (59)</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>B00008 (59)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>B00389 (59)</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>B00423 (59)</t>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>B00401 (57)</t>
+          <t>B00221 (57)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -2290,12 +2290,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
+          <t>B00348 (137)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>B00397 (137)</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>B00348 (137)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -2642,12 +2642,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>T01195 (173)</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>T01013 (173)</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>T01195 (173)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -3145,14 +3145,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>T01018 (102)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>T01158 (102)</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>T01018 (102)</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>T01220 (96)</t>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>B00176 (86)</t>
+          <t>T01288 (86)</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -3743,12 +3743,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>T01362 (151)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>T01177 (151)</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>T01362 (151)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -4095,12 +4095,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
+          <t>T01068 (183)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>B00083 (183)</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>T01068 (183)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -4281,7 +4281,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>T01028 (213)</t>
+          <t>T01238 (213)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -4412,19 +4412,19 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>T01283 (201)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>T01297 (201)</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>B01479 (201)</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>T01283 (201)</t>
-        </is>
-      </c>
       <c r="H7" t="inlineStr">
         <is>
           <t>B01476 (199)</t>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>T01121 (187)</t>
+          <t>T01225 (187)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -4975,17 +4975,17 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
+          <t>T01232 (53)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
           <t>T01146 (53)</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>T01393 (53)</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>T01232 (53)</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -5347,17 +5347,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>T01255 (46)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>T01267 (46)</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>B01484 (46)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>T01255 (46)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -5538,12 +5538,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>T01013 (46)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>B01465 (46)</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>T01013 (46)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -5875,12 +5875,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
+          <t>T01042 (130)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>T01152 (130)</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>T01042 (130)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -6564,12 +6564,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>B00585 (212)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>B01660 (212)</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>B00585 (212)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>T01395 (194)</t>
+          <t>T01093 (194)</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -6921,12 +6921,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>B01795 (160)</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>A07813 (160)</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>B01795 (160)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -7971,12 +7971,12 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
+          <t>822 (29)</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
           <t>1139 (29)</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>822 (29)</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -8152,14 +8152,14 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
+          <t>1302 (61)</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
           <t>660 (61)</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>1302 (61)</t>
-        </is>
-      </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>1086 (60)</t>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>900 (58)</t>
+          <t>769 (58)</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -8373,22 +8373,22 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
+          <t>782 (109)</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
           <t>709 (109)</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>782 (109)</t>
-        </is>
-      </c>
       <c r="V5" t="inlineStr">
         <is>
+          <t>1289 (108)</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
           <t>948 (108)</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>1289 (108)</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
@@ -8569,17 +8569,17 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
+          <t>774 (182)</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>1067 (182)</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
           <t>614 (182)</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>1067 (182)</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>774 (182)</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -8775,14 +8775,14 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
+          <t>1230 (180)</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
           <t>617 (180)</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>1230 (180)</t>
-        </is>
-      </c>
       <c r="T7" t="inlineStr">
         <is>
           <t>404 (173)</t>
@@ -8800,12 +8800,12 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
+          <t>351 (171)</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
           <t>462 (171)</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>351 (171)</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -10011,12 +10011,12 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
+          <t>1418 (152)</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
           <t>1495 (152)</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>1418 (152)</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -10473,24 +10473,24 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
+          <t>1565 (63)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
           <t>654 (63)</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1565 (63)</t>
-        </is>
-      </c>
       <c r="S2" t="inlineStr">
         <is>
+          <t>643 (59)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
           <t>681 (59)</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>643 (59)</t>
-        </is>
-      </c>
       <c r="U2" t="inlineStr">
         <is>
           <t>639 (58)</t>
@@ -10498,12 +10498,12 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
+          <t>1550 (57)</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
           <t>926 (57)</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>1550 (57)</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -10669,12 +10669,12 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>1545 (74)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>653 (74)</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>1545 (74)</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -11317,14 +11317,14 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
+          <t>1443 (224)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
           <t>1384 (224)</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>1443 (224)</t>
-        </is>
-      </c>
       <c r="W6" t="inlineStr">
         <is>
           <t>1591 (219)</t>
@@ -11332,7 +11332,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>1514 (216)</t>
+          <t>1428 (216)</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -11719,14 +11719,14 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
+          <t>1385 (241)</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
           <t>1479 (241)</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>1385 (241)</t>
-        </is>
-      </c>
       <c r="U8" t="inlineStr">
         <is>
           <t>1591 (240)</t>
@@ -11744,7 +11744,7 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>350 (235)</t>
+          <t>1433 (235)</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -11769,12 +11769,12 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
+          <t>Charles Circle - Charles St. at Cambridge St. (2625)</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
           <t>Boston Public Library - 700 Boylston St. (2625)</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>Charles Circle - Charles St. at Cambridge St. (2625)</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
@@ -12342,12 +12342,12 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
+          <t>1810 (195)</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
           <t>1700 (195)</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>1810 (195)</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
@@ -12553,12 +12553,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
+          <t>1880 (155)</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
           <t>1429 (155)</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>1880 (155)</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -13010,12 +13010,12 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
+          <t>1559 (68)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
           <t>1656 (68)</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>1559 (68)</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -13432,12 +13432,12 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
+          <t>769 (74)</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
           <t>1483 (74)</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>769 (74)</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -13623,12 +13623,12 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
+          <t>1434 (148)</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
           <t>277 (148)</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>1434 (148)</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -13844,22 +13844,22 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
+          <t>1711 (165)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>1710 (165)</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>1690 (165)</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
           <t>1811 (165)</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>1711 (165)</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>1690 (165)</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>1710 (165)</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -14030,12 +14030,12 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
+          <t>1865 (211)</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
           <t>1828 (211)</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>1865 (211)</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -14658,12 +14658,12 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
+          <t>1824 (209)</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
           <t>1257 (209)</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>1824 (209)</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -15075,12 +15075,12 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
+          <t>1900 (160)</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
           <t>1749 (160)</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>1900 (160)</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
@@ -15286,12 +15286,12 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
+          <t>1906 (88)</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
           <t>1893 (88)</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>1906 (88)</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">

</xml_diff>